<commit_message>
ADD WHOLE PAGE (MINDMAP) UPDATA  FYP - FEATURES ( AFTER MEETING 1 )
</commit_message>
<xml_diff>
--- a/MENU/PROPOSAL/PLAN/FYP - FEATURES ( AFTER MEETING 1 ) .xlsx
+++ b/MENU/PROPOSAL/PLAN/FYP - FEATURES ( AFTER MEETING 1 ) .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12620"/>
+    <workbookView windowWidth="19200" windowHeight="7210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>PAGE</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Send</t>
+  </si>
+  <si>
+    <t>ACTIVITY PAGE</t>
+  </si>
+  <si>
+    <t>Visit</t>
   </si>
   <si>
     <t>MANAGEMENT PAGE</t>
@@ -203,6 +209,58 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -210,14 +268,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,34 +285,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -274,14 +305,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -290,49 +336,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -346,7 +352,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,12 +367,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -391,73 +391,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -469,19 +547,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,92 +575,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -638,11 +638,66 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -663,39 +718,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -707,15 +729,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -742,10 +755,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -754,137 +767,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -894,67 +907,64 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1276,10 +1286,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:F21"/>
+  <dimension ref="A2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6363636363636" defaultRowHeight="17" customHeight="1" outlineLevelCol="5"/>
@@ -1293,314 +1303,330 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:6">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:6">
-      <c r="A4" s="9"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="10"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" customHeight="1" spans="1:6">
-      <c r="A5" s="9"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
-      <c r="A6" s="9"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:6">
-      <c r="A7" s="9"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="14"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" customHeight="1" spans="1:6">
-      <c r="A8" s="9"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="14"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" customHeight="1" spans="1:6">
-      <c r="A9" s="9"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" customHeight="1" spans="1:6">
-      <c r="A10" s="9"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="10"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" customHeight="1" spans="1:6">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="17" t="s">
+      <c r="E11" s="8"/>
+      <c r="F11" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:6">
-      <c r="A12" s="9"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="18"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" customHeight="1" spans="1:6">
-      <c r="A13" s="9"/>
-      <c r="B13" s="11" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="18"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="15"/>
     </row>
     <row r="14" customHeight="1" spans="1:6">
-      <c r="A14" s="9"/>
-      <c r="B14" s="11" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="18"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" customHeight="1" spans="1:6">
-      <c r="A15" s="9"/>
-      <c r="B15" s="11" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="18"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" customHeight="1" spans="1:6">
-      <c r="A16" s="9"/>
-      <c r="B16" s="11" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="19"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" customHeight="1" spans="1:6">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="E17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" customHeight="1" spans="1:6">
+      <c r="A18" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F18" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" customHeight="1" spans="1:6">
-      <c r="A18" s="9"/>
-      <c r="B18" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="6" t="s">
+    <row r="19" customHeight="1" spans="1:6">
+      <c r="A19" s="16"/>
+      <c r="B19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" customHeight="1" spans="1:6">
-      <c r="A19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="11" t="s">
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" customHeight="1" spans="1:6">
+      <c r="A20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F20" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customHeight="1" spans="1:6">
-      <c r="A20" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="15" t="s">
+    <row r="21" customHeight="1" spans="1:6">
+      <c r="A21" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" customHeight="1" spans="1:6">
-      <c r="A21" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="6" t="s">
+      <c r="F21" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="6" t="s">
+    </row>
+    <row r="22" customHeight="1" spans="1:6">
+      <c r="A22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="C22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F22" s="22" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="15">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
@@ -1611,12 +1637,11 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A11:A17"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="F6:F10"/>
-    <mergeCell ref="F11:F16"/>
-    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F11:F17"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>